<commit_message>
agrego accesorio movilidad para la emisión de varios autos
</commit_message>
<xml_diff>
--- a/Sura/DataSource - ValidaFormularios - Emitida.xlsx
+++ b/Sura/DataSource - ValidaFormularios - Emitida.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC47A804-D3FF-49CF-93D7-7A81F29D6DAF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CD4EE3-C905-49D0-9CAD-57A0745A2467}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>04104016708</t>
-  </si>
-  <si>
     <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>gw</t>
+  </si>
+  <si>
+    <t>04104017645</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,19 +461,19 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>

</xml_diff>